<commit_message>
Added code to import library
</commit_message>
<xml_diff>
--- a/cholesky.xlsx
+++ b/cholesky.xlsx
@@ -557,7 +557,7 @@
         <v>0.0030694793547829</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0109664943115029</v>
+        <v>0.0109664966149075</v>
       </c>
       <c r="J2" t="n">
         <v>0.0198386637035976</v>
@@ -652,7 +652,7 @@
         <v>0.0150934972297941</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0121606921525809</v>
+        <v>0.012160659828565</v>
       </c>
       <c r="J3" t="n">
         <v>0.00953534343740888</v>
@@ -747,7 +747,7 @@
         <v>0.00498490356135304</v>
       </c>
       <c r="I4" t="n">
-        <v>0.00856694959450886</v>
+        <v>0.00856693148983032</v>
       </c>
       <c r="J4" t="n">
         <v>0.00554380766246955</v>
@@ -842,7 +842,7 @@
         <v>0.0150477937331775</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0176300520562803</v>
+        <v>0.0176300649468476</v>
       </c>
       <c r="J5" t="n">
         <v>0.00777622695244366</v>
@@ -937,7 +937,7 @@
         <v>0.00379167923253664</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.00241574506859504</v>
+        <v>-0.00241575720827577</v>
       </c>
       <c r="J6" t="n">
         <v>0.00665675055161459</v>
@@ -1032,7 +1032,7 @@
         <v>-0.0114421554175681</v>
       </c>
       <c r="I7" t="n">
-        <v>0.00224480911839096</v>
+        <v>0.00224481745645716</v>
       </c>
       <c r="J7" t="n">
         <v>-0.00383059112463069</v>
@@ -1127,7 +1127,7 @@
         <v>0.0516219569078682</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0144784103545241</v>
+        <v>0.0144784201237608</v>
       </c>
       <c r="J8" t="n">
         <v>0.00852623015255662</v>
@@ -1222,73 +1222,73 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0408511085709444</v>
+        <v>0.0408511112412288</v>
       </c>
       <c r="J9" t="n">
-        <v>0.00921938988584798</v>
+        <v>0.00921938391665778</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.00428861620616036</v>
+        <v>-0.00428864551232178</v>
       </c>
       <c r="L9" t="n">
-        <v>0.00393684245251702</v>
+        <v>0.00393687546096538</v>
       </c>
       <c r="M9" t="n">
-        <v>0.0115667867494143</v>
+        <v>0.0115668076149246</v>
       </c>
       <c r="N9" t="n">
-        <v>0.0172219059079589</v>
+        <v>0.0172219087521292</v>
       </c>
       <c r="O9" t="n">
-        <v>0.0056028127119746</v>
+        <v>0.00560283241676823</v>
       </c>
       <c r="P9" t="n">
-        <v>-0.00820708358134253</v>
+        <v>-0.00820705264961571</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.000848073165078921</v>
+        <v>0.000848073745140224</v>
       </c>
       <c r="R9" t="n">
-        <v>0.0212850621868535</v>
+        <v>0.0212850866919606</v>
       </c>
       <c r="S9" t="n">
-        <v>-0.0184963183076198</v>
+        <v>-0.0184962623103979</v>
       </c>
       <c r="T9" t="n">
-        <v>-0.000963621917589186</v>
+        <v>-0.000963730287763449</v>
       </c>
       <c r="U9" t="n">
-        <v>-0.000325693767514596</v>
+        <v>-0.000325739820785986</v>
       </c>
       <c r="V9" t="n">
-        <v>-0.0142912065681403</v>
+        <v>-0.0142912373482396</v>
       </c>
       <c r="W9" t="n">
-        <v>0.0150738542257533</v>
+        <v>0.0150738081291856</v>
       </c>
       <c r="X9" t="n">
-        <v>0.00942378609785397</v>
+        <v>0.00942373587348585</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.0193878477161719</v>
+        <v>0.0193878618092436</v>
       </c>
       <c r="Z9" t="n">
-        <v>-0.00344124125406533</v>
+        <v>-0.00344120673904846</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.0114968068561988</v>
+        <v>0.011496815128907</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.00659632495724572</v>
+        <v>0.00659628216924776</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.0278456693747916</v>
+        <v>0.0278456248625184</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.00236061791516681</v>
+        <v>0.00236064279675913</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.003719218681201</v>
+        <v>0.00371922725150855</v>
       </c>
     </row>
     <row r="10">
@@ -1320,70 +1320,70 @@
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0298025752049502</v>
+        <v>0.0298025770515112</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.0101862641066196</v>
+        <v>-0.0101862552686341</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.00208958601131775</v>
+        <v>-0.00208959530444861</v>
       </c>
       <c r="M10" t="n">
-        <v>0.0146125580342196</v>
+        <v>0.0146125529908377</v>
       </c>
       <c r="N10" t="n">
-        <v>0.0129724028327033</v>
+        <v>0.0129724045984902</v>
       </c>
       <c r="O10" t="n">
-        <v>0.0191370870260599</v>
+        <v>0.0191370808668744</v>
       </c>
       <c r="P10" t="n">
-        <v>0.00131558081738459</v>
+        <v>0.00131556952338114</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.00335670811648403</v>
+        <v>0.00335670789892352</v>
       </c>
       <c r="R10" t="n">
-        <v>-0.00280400605658312</v>
+        <v>-0.00280400920025884</v>
       </c>
       <c r="S10" t="n">
-        <v>-0.0115308700425484</v>
+        <v>-0.0115308903554051</v>
       </c>
       <c r="T10" t="n">
-        <v>0.0147471607659308</v>
+        <v>0.0147471931833512</v>
       </c>
       <c r="U10" t="n">
-        <v>0.00816439702952575</v>
+        <v>0.00816441070494059</v>
       </c>
       <c r="V10" t="n">
-        <v>0.0209295183313419</v>
+        <v>0.0209295236939315</v>
       </c>
       <c r="W10" t="n">
-        <v>-0.000000520380274276847</v>
+        <v>-0.00000050310117730155</v>
       </c>
       <c r="X10" t="n">
-        <v>0.00147508539010049</v>
+        <v>0.00147510272304009</v>
       </c>
       <c r="Y10" t="n">
-        <v>-0.0103660338781267</v>
+        <v>-0.0103660337123079</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.00150638794084677</v>
+        <v>0.00150637648109107</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.0078279030670984</v>
+        <v>0.00782790232564083</v>
       </c>
       <c r="AB10" t="n">
-        <v>-0.00226704251575324</v>
+        <v>-0.00226702781769777</v>
       </c>
       <c r="AC10" t="n">
-        <v>-0.00557222816457804</v>
+        <v>-0.00557220847227795</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.00824727790616707</v>
+        <v>0.00824727017089385</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.0046035212809926</v>
+        <v>0.00460351908947358</v>
       </c>
     </row>
     <row r="11">
@@ -1418,67 +1418,67 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>0.0704906271767767</v>
+        <v>0.0704906266709323</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0131909920310039</v>
+        <v>0.0131909946897034</v>
       </c>
       <c r="M11" t="n">
-        <v>0.0145301960273988</v>
+        <v>0.0145301996490741</v>
       </c>
       <c r="N11" t="n">
-        <v>0.00686352928249478</v>
+        <v>0.00686353529342615</v>
       </c>
       <c r="O11" t="n">
-        <v>-0.00578560747251766</v>
+        <v>-0.00578560727525943</v>
       </c>
       <c r="P11" t="n">
-        <v>0.00463243116314443</v>
+        <v>0.00463242786922704</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.0132747682060581</v>
+        <v>0.0132747682368955</v>
       </c>
       <c r="R11" t="n">
-        <v>0.0198374357380815</v>
+        <v>0.0198374461177782</v>
       </c>
       <c r="S11" t="n">
-        <v>-0.00438669522498085</v>
+        <v>-0.00438670102894572</v>
       </c>
       <c r="T11" t="n">
-        <v>0.00708844845963394</v>
+        <v>0.0070884443521553</v>
       </c>
       <c r="U11" t="n">
-        <v>0.00638780865665997</v>
+        <v>0.00638780671774532</v>
       </c>
       <c r="V11" t="n">
-        <v>0.0162531858179386</v>
+        <v>0.0162531762712249</v>
       </c>
       <c r="W11" t="n">
-        <v>-0.0012603316382091</v>
+        <v>-0.0012603256878956</v>
       </c>
       <c r="X11" t="n">
-        <v>-0.00149720692801048</v>
+        <v>-0.0014972037567506</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.00801834348284998</v>
+        <v>0.00801835378185826</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.00677131744221748</v>
+        <v>0.00677131631515844</v>
       </c>
       <c r="AA11" t="n">
-        <v>-0.0114244000766892</v>
+        <v>-0.0114243959642069</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.00816379522485148</v>
+        <v>0.0081637978307902</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.0124305535624727</v>
+        <v>0.0124305660645366</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.00530245574219551</v>
+        <v>0.00530245612364205</v>
       </c>
       <c r="AE11" t="n">
-        <v>0.00721008704992779</v>
+        <v>0.00721008827546648</v>
       </c>
     </row>
     <row r="12">
@@ -1516,64 +1516,64 @@
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>0.0373468385370319</v>
+        <v>0.0373468335984788</v>
       </c>
       <c r="M12" t="n">
-        <v>-0.000297106604241653</v>
+        <v>-0.000297118025852852</v>
       </c>
       <c r="N12" t="n">
-        <v>-0.00254305462003687</v>
+        <v>-0.00254306976238497</v>
       </c>
       <c r="O12" t="n">
-        <v>0.00752466869158866</v>
+        <v>0.0075246674170204</v>
       </c>
       <c r="P12" t="n">
-        <v>0.00977484222788289</v>
+        <v>0.00977484804262184</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.00388522022019371</v>
+        <v>0.00388521979042439</v>
       </c>
       <c r="R12" t="n">
-        <v>0.00191774092636004</v>
+        <v>0.00191771383231278</v>
       </c>
       <c r="S12" t="n">
-        <v>0.00312409169487786</v>
+        <v>0.00312410090927646</v>
       </c>
       <c r="T12" t="n">
-        <v>-0.00616508288807142</v>
+        <v>-0.00616506499838307</v>
       </c>
       <c r="U12" t="n">
-        <v>-0.0130989300130918</v>
+        <v>-0.0130989235759003</v>
       </c>
       <c r="V12" t="n">
-        <v>0.0201984226353402</v>
+        <v>0.0201984489048674</v>
       </c>
       <c r="W12" t="n">
-        <v>0.00455702563205182</v>
+        <v>0.00455701672577587</v>
       </c>
       <c r="X12" t="n">
-        <v>-0.00173864218162034</v>
+        <v>-0.00173864512292215</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.0113671984377669</v>
+        <v>0.0113671745410457</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.0100286552409483</v>
+        <v>0.0100286556199014</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.00716609589000563</v>
+        <v>0.00716608707138557</v>
       </c>
       <c r="AB12" t="n">
-        <v>-0.00168658886689968</v>
+        <v>-0.0016865916528836</v>
       </c>
       <c r="AC12" t="n">
-        <v>-0.00110731074150524</v>
+        <v>-0.00110733639213626</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.0067025187577518</v>
+        <v>0.00670251604198814</v>
       </c>
       <c r="AE12" t="n">
-        <v>-0.00500211254820458</v>
+        <v>-0.00500211732351866</v>
       </c>
     </row>
     <row r="13">
@@ -1614,61 +1614,61 @@
         <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>0.0819960957990025</v>
+        <v>0.0819960930712191</v>
       </c>
       <c r="N13" t="n">
-        <v>0.0127165957668146</v>
+        <v>0.0127165901119851</v>
       </c>
       <c r="O13" t="n">
-        <v>0.0146123939248984</v>
+        <v>0.0146123937444257</v>
       </c>
       <c r="P13" t="n">
-        <v>-0.003357276262757</v>
+        <v>-0.00335727479401436</v>
       </c>
       <c r="Q13" t="n">
-        <v>-0.000010292958735926</v>
+        <v>-0.0000102930636425087</v>
       </c>
       <c r="R13" t="n">
-        <v>0.00840911223108235</v>
+        <v>0.00840910147878826</v>
       </c>
       <c r="S13" t="n">
-        <v>0.0115972570481318</v>
+        <v>0.011597258842959</v>
       </c>
       <c r="T13" t="n">
-        <v>-0.00549488134784008</v>
+        <v>-0.00549487124736542</v>
       </c>
       <c r="U13" t="n">
-        <v>0.00227096007472201</v>
+        <v>0.00227096305490303</v>
       </c>
       <c r="V13" t="n">
-        <v>0.022076175176424</v>
+        <v>0.0220761881037452</v>
       </c>
       <c r="W13" t="n">
-        <v>0.0022683256329152</v>
+        <v>0.00226832489955411</v>
       </c>
       <c r="X13" t="n">
-        <v>-0.00179764202768715</v>
+        <v>-0.00179764114749656</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.00768272297883228</v>
+        <v>0.00768271496320412</v>
       </c>
       <c r="Z13" t="n">
-        <v>-0.000811964992186001</v>
+        <v>-0.000811965578527576</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.00774146185125249</v>
+        <v>0.00774145937191031</v>
       </c>
       <c r="AB13" t="n">
-        <v>-0.000600919629438674</v>
+        <v>-0.00060091911827717</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.00523925131027259</v>
+        <v>0.00523924381405248</v>
       </c>
       <c r="AD13" t="n">
-        <v>0.00365158117488141</v>
+        <v>0.00365157969348509</v>
       </c>
       <c r="AE13" t="n">
-        <v>-0.00177547780400244</v>
+        <v>-0.00177548059447127</v>
       </c>
     </row>
     <row r="14">
@@ -1712,58 +1712,58 @@
         <v>0</v>
       </c>
       <c r="N14" t="n">
-        <v>0.0349267645603102</v>
+        <v>0.0349267622771749</v>
       </c>
       <c r="O14" t="n">
-        <v>0.00581601867257143</v>
+        <v>0.00581601675842627</v>
       </c>
       <c r="P14" t="n">
-        <v>-0.000222426849126753</v>
+        <v>-0.000222433886128795</v>
       </c>
       <c r="Q14" t="n">
-        <v>-0.00700798898049621</v>
+        <v>-0.00700799048358613</v>
       </c>
       <c r="R14" t="n">
-        <v>0.0102978509880003</v>
+        <v>0.0102978378353188</v>
       </c>
       <c r="S14" t="n">
-        <v>-0.0199999334906944</v>
+        <v>-0.0199999476307985</v>
       </c>
       <c r="T14" t="n">
-        <v>0.0000722941805228306</v>
+        <v>0.0000723285634151471</v>
       </c>
       <c r="U14" t="n">
-        <v>0.00665153316319687</v>
+        <v>0.00665154419471659</v>
       </c>
       <c r="V14" t="n">
-        <v>-0.0143188817872628</v>
+        <v>-0.0143188608161302</v>
       </c>
       <c r="W14" t="n">
-        <v>0.010845327777203</v>
+        <v>0.0108453445795713</v>
       </c>
       <c r="X14" t="n">
-        <v>0.00417935114768205</v>
+        <v>0.00417936696111963</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.00627045151006305</v>
+        <v>0.00627044780124996</v>
       </c>
       <c r="Z14" t="n">
-        <v>-0.00619464128793377</v>
+        <v>-0.00619465073770898</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.0141077867736164</v>
+        <v>0.014107788338922</v>
       </c>
       <c r="AB14" t="n">
-        <v>0.0096651913677115</v>
+        <v>0.00966520408147783</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.0156071151567248</v>
+        <v>0.0156071254591902</v>
       </c>
       <c r="AD14" t="n">
-        <v>0.00159381884949898</v>
+        <v>0.00159381179990926</v>
       </c>
       <c r="AE14" t="n">
-        <v>0.0105891616354086</v>
+        <v>0.0105891551105681</v>
       </c>
     </row>
     <row r="15">
@@ -1810,55 +1810,55 @@
         <v>0</v>
       </c>
       <c r="O15" t="n">
-        <v>0.0319545480482502</v>
+        <v>0.0319545490486771</v>
       </c>
       <c r="P15" t="n">
-        <v>-0.00795032239721484</v>
+        <v>-0.00795031652099554</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.00962947447822077</v>
+        <v>0.00962947441087058</v>
       </c>
       <c r="R15" t="n">
-        <v>0.0068553995881363</v>
+        <v>0.00685539948224202</v>
       </c>
       <c r="S15" t="n">
-        <v>0.0124554539808838</v>
+        <v>0.012455462672145</v>
       </c>
       <c r="T15" t="n">
-        <v>-0.00369898156774251</v>
+        <v>-0.00369899457769019</v>
       </c>
       <c r="U15" t="n">
-        <v>-0.0192844761181211</v>
+        <v>-0.0192844792431401</v>
       </c>
       <c r="V15" t="n">
-        <v>-0.0205159205770247</v>
+        <v>-0.020515922573187</v>
       </c>
       <c r="W15" t="n">
-        <v>0.00166578372570524</v>
+        <v>0.00166577341621793</v>
       </c>
       <c r="X15" t="n">
-        <v>-0.00638048211593103</v>
+        <v>-0.00638049085104189</v>
       </c>
       <c r="Y15" t="n">
-        <v>-0.00900958362357463</v>
+        <v>-0.00900958721011394</v>
       </c>
       <c r="Z15" t="n">
-        <v>-0.00831713724812806</v>
+        <v>-0.00831713208672238</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.014825713084542</v>
+        <v>0.0148257109484572</v>
       </c>
       <c r="AB15" t="n">
-        <v>-0.00916370130835067</v>
+        <v>-0.0091637077881413</v>
       </c>
       <c r="AC15" t="n">
-        <v>0.0107180503440904</v>
+        <v>0.0107180384748836</v>
       </c>
       <c r="AD15" t="n">
-        <v>-0.00481884640468899</v>
+        <v>-0.00481884283020076</v>
       </c>
       <c r="AE15" t="n">
-        <v>0.000400726202567334</v>
+        <v>0.000400728783921816</v>
       </c>
     </row>
     <row r="16">
@@ -1908,52 +1908,52 @@
         <v>0</v>
       </c>
       <c r="P16" t="n">
-        <v>0.0350051649049103</v>
+        <v>0.0350051728243441</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.0130280727565014</v>
+        <v>0.0130280679468028</v>
       </c>
       <c r="R16" t="n">
-        <v>0.00893237954902056</v>
+        <v>0.00893237084667848</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.00923257150540949</v>
+        <v>-0.00923255017936181</v>
       </c>
       <c r="T16" t="n">
-        <v>0.0110868756964598</v>
+        <v>0.0110868485092762</v>
       </c>
       <c r="U16" t="n">
-        <v>0.000809176516206453</v>
+        <v>0.000809173305100192</v>
       </c>
       <c r="V16" t="n">
-        <v>0.0266596271296923</v>
+        <v>0.0266596257221498</v>
       </c>
       <c r="W16" t="n">
-        <v>0.00127363597504054</v>
+        <v>0.00127361123447931</v>
       </c>
       <c r="X16" t="n">
-        <v>0.0054973795089277</v>
+        <v>0.00549735872457342</v>
       </c>
       <c r="Y16" t="n">
-        <v>0.00512405937399553</v>
+        <v>0.00512404605644384</v>
       </c>
       <c r="Z16" t="n">
-        <v>0.0106092325402152</v>
+        <v>0.0106092424452008</v>
       </c>
       <c r="AA16" t="n">
-        <v>0.0118057546316459</v>
+        <v>0.0118057452572092</v>
       </c>
       <c r="AB16" t="n">
-        <v>0.00450134190051095</v>
+        <v>0.00450132738389691</v>
       </c>
       <c r="AC16" t="n">
-        <v>0.00348171567176094</v>
+        <v>0.0034816819358796</v>
       </c>
       <c r="AD16" t="n">
-        <v>0.0015619680481948</v>
+        <v>0.00156197608858339</v>
       </c>
       <c r="AE16" t="n">
-        <v>0.0000573159631948601</v>
+        <v>0.0000573213345274508</v>
       </c>
     </row>
     <row r="17">
@@ -2006,49 +2006,49 @@
         <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.0415281806519055</v>
+        <v>0.0415281819588171</v>
       </c>
       <c r="R17" t="n">
-        <v>0.00437154554274091</v>
+        <v>0.00437154604084775</v>
       </c>
       <c r="S17" t="n">
-        <v>-0.0306279988250056</v>
+        <v>-0.0306280089711175</v>
       </c>
       <c r="T17" t="n">
-        <v>0.0123703675716803</v>
+        <v>0.0123703850534177</v>
       </c>
       <c r="U17" t="n">
-        <v>0.00772880005978871</v>
+        <v>0.00772880347949495</v>
       </c>
       <c r="V17" t="n">
-        <v>0.0346916996395534</v>
+        <v>0.0346917068815959</v>
       </c>
       <c r="W17" t="n">
-        <v>-0.000984846004579654</v>
+        <v>-0.000984834124353576</v>
       </c>
       <c r="X17" t="n">
-        <v>-0.00347632344170568</v>
+        <v>-0.00347631259925367</v>
       </c>
       <c r="Y17" t="n">
-        <v>-0.000425028213570821</v>
+        <v>-0.000425024564371128</v>
       </c>
       <c r="Z17" t="n">
-        <v>-0.00412181507946585</v>
+        <v>-0.00412181915878817</v>
       </c>
       <c r="AA17" t="n">
-        <v>0.00211489804906605</v>
+        <v>0.00211490296831893</v>
       </c>
       <c r="AB17" t="n">
-        <v>-0.00259376133106978</v>
+        <v>-0.00259375320656012</v>
       </c>
       <c r="AC17" t="n">
-        <v>-0.00496094796637516</v>
+        <v>-0.00496093445721315</v>
       </c>
       <c r="AD17" t="n">
-        <v>-0.00379050865999885</v>
+        <v>-0.00379051251703962</v>
       </c>
       <c r="AE17" t="n">
-        <v>-0.0025976953500741</v>
+        <v>-0.00259769829548546</v>
       </c>
     </row>
     <row r="18">
@@ -2104,46 +2104,46 @@
         <v>0</v>
       </c>
       <c r="R18" t="n">
-        <v>0.0453345496512276</v>
+        <v>0.0453345412202828</v>
       </c>
       <c r="S18" t="n">
-        <v>0.00803179014201641</v>
+        <v>0.00803177219043735</v>
       </c>
       <c r="T18" t="n">
-        <v>-0.00672320667494985</v>
+        <v>-0.00672316110653315</v>
       </c>
       <c r="U18" t="n">
-        <v>0.00410371386445134</v>
+        <v>0.00410372933388935</v>
       </c>
       <c r="V18" t="n">
-        <v>0.0364278006971518</v>
+        <v>0.0364278413371739</v>
       </c>
       <c r="W18" t="n">
-        <v>-0.00579655839589099</v>
+        <v>-0.00579653857415523</v>
       </c>
       <c r="X18" t="n">
-        <v>-0.00185629984560998</v>
+        <v>-0.00185628000905103</v>
       </c>
       <c r="Y18" t="n">
-        <v>0.0061484112548515</v>
+        <v>0.0061484058072459</v>
       </c>
       <c r="Z18" t="n">
-        <v>-0.000991486595342041</v>
+        <v>-0.00099149681959634</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.00440017051890831</v>
+        <v>0.00440017721434505</v>
       </c>
       <c r="AB18" t="n">
-        <v>0.00826970363897259</v>
+        <v>0.0082697221597211</v>
       </c>
       <c r="AC18" t="n">
-        <v>-0.00872884391488868</v>
+        <v>-0.00872883404470257</v>
       </c>
       <c r="AD18" t="n">
-        <v>0.00317650812034087</v>
+        <v>0.0031765003680104</v>
       </c>
       <c r="AE18" t="n">
-        <v>0.00935357471409996</v>
+        <v>0.00935356915510802</v>
       </c>
     </row>
     <row r="19">
@@ -2202,43 +2202,43 @@
         <v>0</v>
       </c>
       <c r="S19" t="n">
-        <v>0.0904570736713066</v>
+        <v>0.0904570777143394</v>
       </c>
       <c r="T19" t="n">
-        <v>-0.00854728865417729</v>
+        <v>-0.00854729701307307</v>
       </c>
       <c r="U19" t="n">
-        <v>-0.0139396857607884</v>
+        <v>-0.0139396830664517</v>
       </c>
       <c r="V19" t="n">
-        <v>0.0169867233056679</v>
+        <v>0.0169867341823844</v>
       </c>
       <c r="W19" t="n">
-        <v>0.0033460724543868</v>
+        <v>0.00334606069651919</v>
       </c>
       <c r="X19" t="n">
-        <v>-0.00366019679187075</v>
+        <v>-0.003660206232143</v>
       </c>
       <c r="Y19" t="n">
-        <v>-0.00208181213961005</v>
+        <v>-0.00208182007279793</v>
       </c>
       <c r="Z19" t="n">
-        <v>-0.00564589617503812</v>
+        <v>-0.00564589401302626</v>
       </c>
       <c r="AA19" t="n">
-        <v>0.000659736863210136</v>
+        <v>0.000659732139294975</v>
       </c>
       <c r="AB19" t="n">
-        <v>0.00755955282469196</v>
+        <v>0.00755954789171157</v>
       </c>
       <c r="AC19" t="n">
-        <v>0.00714578818084173</v>
+        <v>0.00714576850755052</v>
       </c>
       <c r="AD19" t="n">
-        <v>0.00368671260891163</v>
+        <v>0.00368671552496134</v>
       </c>
       <c r="AE19" t="n">
-        <v>-0.000759270465338427</v>
+        <v>-0.000759267222856666</v>
       </c>
     </row>
     <row r="20">
@@ -2300,40 +2300,40 @@
         <v>0</v>
       </c>
       <c r="T20" t="n">
-        <v>0.0418042120429975</v>
+        <v>0.0418042092175036</v>
       </c>
       <c r="U20" t="n">
-        <v>0.00153202231584788</v>
+        <v>0.00153199785657543</v>
       </c>
       <c r="V20" t="n">
-        <v>-0.00872238520998391</v>
+        <v>-0.00872246817840558</v>
       </c>
       <c r="W20" t="n">
-        <v>0.00414504144864089</v>
+        <v>0.00414507132108289</v>
       </c>
       <c r="X20" t="n">
-        <v>0.00430672213367951</v>
+        <v>0.00430674227451839</v>
       </c>
       <c r="Y20" t="n">
-        <v>0.00608850500885001</v>
+        <v>0.00608853980154843</v>
       </c>
       <c r="Z20" t="n">
-        <v>-0.0056538516430143</v>
+        <v>-0.005653851603289</v>
       </c>
       <c r="AA20" t="n">
-        <v>0.00334301229046287</v>
+        <v>0.00334302440793533</v>
       </c>
       <c r="AB20" t="n">
-        <v>0.00256662193792785</v>
+        <v>0.00256662420988235</v>
       </c>
       <c r="AC20" t="n">
-        <v>-0.00249092047190639</v>
+        <v>-0.00249085133770909</v>
       </c>
       <c r="AD20" t="n">
-        <v>-0.000993775593241716</v>
+        <v>-0.000993780771517302</v>
       </c>
       <c r="AE20" t="n">
-        <v>0.00364658839866589</v>
+        <v>0.00364657933362274</v>
       </c>
     </row>
     <row r="21">
@@ -2398,37 +2398,37 @@
         <v>0</v>
       </c>
       <c r="U21" t="n">
-        <v>0.0411901253111125</v>
+        <v>0.0411901208770609</v>
       </c>
       <c r="V21" t="n">
-        <v>0.0237410843793091</v>
+        <v>0.0237410464049858</v>
       </c>
       <c r="W21" t="n">
-        <v>0.00573873639037211</v>
+        <v>0.00573873089626591</v>
       </c>
       <c r="X21" t="n">
-        <v>0.0114363667953728</v>
+        <v>0.0114363615141341</v>
       </c>
       <c r="Y21" t="n">
-        <v>0.0127861461646744</v>
+        <v>0.0127861566035277</v>
       </c>
       <c r="Z21" t="n">
-        <v>0.00227903767631904</v>
+        <v>0.00227904110004835</v>
       </c>
       <c r="AA21" t="n">
-        <v>-0.00181571327742985</v>
+        <v>-0.00181571485601299</v>
       </c>
       <c r="AB21" t="n">
-        <v>-0.00110957794723181</v>
+        <v>-0.00110958853643117</v>
       </c>
       <c r="AC21" t="n">
-        <v>0.0160633959822125</v>
+        <v>0.0160633964787543</v>
       </c>
       <c r="AD21" t="n">
-        <v>-0.00136195765574305</v>
+        <v>-0.00136195512512267</v>
       </c>
       <c r="AE21" t="n">
-        <v>-0.00167179343155322</v>
+        <v>-0.00167178997020876</v>
       </c>
     </row>
     <row r="22">
@@ -2496,34 +2496,34 @@
         <v>0</v>
       </c>
       <c r="V22" t="n">
-        <v>0.0984165717581737</v>
+        <v>0.0984165447845297</v>
       </c>
       <c r="W22" t="n">
-        <v>-0.00613990242831217</v>
+        <v>-0.00613990337082539</v>
       </c>
       <c r="X22" t="n">
-        <v>-0.0062763995415468</v>
+        <v>-0.00627640077342055</v>
       </c>
       <c r="Y22" t="n">
-        <v>-0.005692969905702</v>
+        <v>-0.00569294976200457</v>
       </c>
       <c r="Z22" t="n">
-        <v>-0.0128683391679619</v>
+        <v>-0.0128683382801803</v>
       </c>
       <c r="AA22" t="n">
-        <v>-0.0030662650069378</v>
+        <v>-0.00306626575501103</v>
       </c>
       <c r="AB22" t="n">
-        <v>0.0103543189638436</v>
+        <v>0.0103543098115571</v>
       </c>
       <c r="AC22" t="n">
-        <v>0.00418120784179221</v>
+        <v>0.00418122641360471</v>
       </c>
       <c r="AD22" t="n">
-        <v>-0.0021805495109975</v>
+        <v>-0.00218054851005547</v>
       </c>
       <c r="AE22" t="n">
-        <v>-0.00811022205979042</v>
+        <v>-0.00811022236242247</v>
       </c>
     </row>
     <row r="23">
@@ -2594,31 +2594,31 @@
         <v>0</v>
       </c>
       <c r="W23" t="n">
-        <v>0.0252325474970111</v>
+        <v>0.0252325744037335</v>
       </c>
       <c r="X23" t="n">
-        <v>0.017989182806971</v>
+        <v>0.0179892073321517</v>
       </c>
       <c r="Y23" t="n">
-        <v>0.00341940070355349</v>
+        <v>0.00341942524009299</v>
       </c>
       <c r="Z23" t="n">
-        <v>0.0107505270439937</v>
+        <v>0.0107505072739926</v>
       </c>
       <c r="AA23" t="n">
-        <v>0.00192877841328654</v>
+        <v>0.00192879463694618</v>
       </c>
       <c r="AB23" t="n">
-        <v>0.00652463738413287</v>
+        <v>0.00652465795807987</v>
       </c>
       <c r="AC23" t="n">
-        <v>0.0243032420320855</v>
+        <v>0.0243033131917865</v>
       </c>
       <c r="AD23" t="n">
-        <v>-0.00775013829135066</v>
+        <v>-0.00775014346641497</v>
       </c>
       <c r="AE23" t="n">
-        <v>0.0019646450254728</v>
+        <v>0.00196462198489653</v>
       </c>
     </row>
     <row r="24">
@@ -2692,28 +2692,28 @@
         <v>0</v>
       </c>
       <c r="X24" t="n">
-        <v>0.0274444542345896</v>
+        <v>0.0274444544562742</v>
       </c>
       <c r="Y24" t="n">
-        <v>-0.000271059931021704</v>
+        <v>-0.00027105694446533</v>
       </c>
       <c r="Z24" t="n">
-        <v>0.00967878607756051</v>
+        <v>0.00967878298412962</v>
       </c>
       <c r="AA24" t="n">
-        <v>-0.00423613049169421</v>
+        <v>-0.00423612920200111</v>
       </c>
       <c r="AB24" t="n">
-        <v>-0.00581031612166304</v>
+        <v>-0.00581031510030059</v>
       </c>
       <c r="AC24" t="n">
-        <v>0.00451331432493777</v>
+        <v>0.00451331973845422</v>
       </c>
       <c r="AD24" t="n">
-        <v>-0.013410981051415</v>
+        <v>-0.0134109806747351</v>
       </c>
       <c r="AE24" t="n">
-        <v>-0.00306083792166322</v>
+        <v>-0.00306084038272458</v>
       </c>
     </row>
     <row r="25">
@@ -2790,25 +2790,25 @@
         <v>0</v>
       </c>
       <c r="Y25" t="n">
-        <v>0.0345723843375324</v>
+        <v>0.0345723769071292</v>
       </c>
       <c r="Z25" t="n">
-        <v>-0.00329488999346714</v>
+        <v>-0.00329489723453897</v>
       </c>
       <c r="AA25" t="n">
-        <v>0.00631258845782255</v>
+        <v>0.00631259493137801</v>
       </c>
       <c r="AB25" t="n">
-        <v>-0.00483037145788876</v>
+        <v>-0.00483036294074898</v>
       </c>
       <c r="AC25" t="n">
-        <v>-0.0106738646929864</v>
+        <v>-0.0106738800329989</v>
       </c>
       <c r="AD25" t="n">
-        <v>0.00834424745210736</v>
+        <v>0.00834425154554109</v>
       </c>
       <c r="AE25" t="n">
-        <v>-0.000122174234090214</v>
+        <v>-0.000122177435187206</v>
       </c>
     </row>
     <row r="26">
@@ -2888,22 +2888,22 @@
         <v>0</v>
       </c>
       <c r="Z26" t="n">
-        <v>0.0471375610686094</v>
+        <v>0.0471375658719658</v>
       </c>
       <c r="AA26" t="n">
-        <v>0.0183665770887401</v>
+        <v>0.0183665716137195</v>
       </c>
       <c r="AB26" t="n">
-        <v>-0.0133069476491705</v>
+        <v>-0.0133069518417184</v>
       </c>
       <c r="AC26" t="n">
-        <v>-0.00186121930374166</v>
+        <v>-0.00186123384351605</v>
       </c>
       <c r="AD26" t="n">
-        <v>-0.0000484821310859316</v>
+        <v>-0.0000484825049293433</v>
       </c>
       <c r="AE26" t="n">
-        <v>-0.00229399697495088</v>
+        <v>-0.00229398928397952</v>
       </c>
     </row>
     <row r="27">
@@ -2986,19 +2986,19 @@
         <v>0</v>
       </c>
       <c r="AA27" t="n">
-        <v>0.0261305724117716</v>
+        <v>0.0261305766891539</v>
       </c>
       <c r="AB27" t="n">
-        <v>0.00370879922888158</v>
+        <v>0.00370880159382364</v>
       </c>
       <c r="AC27" t="n">
-        <v>-0.0161582363429603</v>
+        <v>-0.0161582041833013</v>
       </c>
       <c r="AD27" t="n">
-        <v>0.00160203018981677</v>
+        <v>0.00160202862025249</v>
       </c>
       <c r="AE27" t="n">
-        <v>-0.000378545455524439</v>
+        <v>-0.000378557285042175</v>
       </c>
     </row>
     <row r="28">
@@ -3084,16 +3084,16 @@
         <v>0</v>
       </c>
       <c r="AB28" t="n">
-        <v>0.039389753769654</v>
+        <v>0.0393897538622146</v>
       </c>
       <c r="AC28" t="n">
-        <v>0.00408220386541444</v>
+        <v>0.00408221070827308</v>
       </c>
       <c r="AD28" t="n">
-        <v>-0.00286234589475645</v>
+        <v>-0.00286234642368812</v>
       </c>
       <c r="AE28" t="n">
-        <v>-0.00314786250967588</v>
+        <v>-0.003147864544861</v>
       </c>
     </row>
     <row r="29">
@@ -3182,13 +3182,13 @@
         <v>0</v>
       </c>
       <c r="AC29" t="n">
-        <v>0.0362686314180473</v>
+        <v>0.0362686373719789</v>
       </c>
       <c r="AD29" t="n">
-        <v>0.000386716168044059</v>
+        <v>0.000386723349075363</v>
       </c>
       <c r="AE29" t="n">
-        <v>-0.00105162275698276</v>
+        <v>-0.0010516378307181</v>
       </c>
     </row>
     <row r="30">
@@ -3280,10 +3280,10 @@
         <v>0</v>
       </c>
       <c r="AD30" t="n">
-        <v>0.0265581135772957</v>
+        <v>0.0265581124959038</v>
       </c>
       <c r="AE30" t="n">
-        <v>0.00184843899329956</v>
+        <v>0.00184843835668443</v>
       </c>
     </row>
     <row r="31">
@@ -3378,7 +3378,7 @@
         <v>0</v>
       </c>
       <c r="AE31" t="n">
-        <v>0.0147202814189448</v>
+        <v>0.0147202896326434</v>
       </c>
     </row>
   </sheetData>

</xml_diff>